<commit_message>
tweak data source names
</commit_message>
<xml_diff>
--- a/1. data/Barkley Sockeye time series of returns.xlsx
+++ b/1. data/Barkley Sockeye time series of returns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\Barkley-Sk-CSAS\1. data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://086gc.sharepoint.com/sites/SalmonScienceStrategy-salmonFSAR/Shared Documents/salmon FSAR - sprint week/Barkley Sockeye/3. Data/Stock-recruit data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B9AD97-FBBF-4333-8282-76AB4F193780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="758" documentId="13_ncr:1_{3A0DAE0A-5A1E-485E-89C6-BA3AF7C7CFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2EF2ED4-E85B-4F51-8ED5-A839A73EFB37}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data sources notes" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5041" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5041" uniqueCount="117">
   <si>
     <t>GCL</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>R-OUT_2024_Area23_full-sk-biodata_2024-11-19.csv (N. Brown)</t>
+  </si>
+  <si>
+    <t>hatchery reports</t>
   </si>
 </sst>
 </file>
@@ -1046,9 +1049,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J663"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H100" sqref="H86:H100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H667" sqref="H667"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2548,7 +2551,7 @@
         <v>18227.413567931726</v>
       </c>
       <c r="G100" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H100" t="s">
         <v>78</v>
@@ -2580,7 +2583,7 @@
         <v>331492.68240361265</v>
       </c>
       <c r="G101" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H101" t="s">
         <v>78</v>
@@ -2612,7 +2615,7 @@
         <v>2584.2883441252047</v>
       </c>
       <c r="G102" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H102" t="s">
         <v>78</v>
@@ -2644,7 +2647,7 @@
         <v>332408.81384317484</v>
       </c>
       <c r="G103" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H103" t="s">
         <v>78</v>
@@ -2676,7 +2679,7 @@
         <v>74698.732955407017</v>
       </c>
       <c r="G104" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H104" t="s">
         <v>78</v>
@@ -2708,7 +2711,7 @@
         <v>34892.425560700605</v>
       </c>
       <c r="G105" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H105" t="s">
         <v>78</v>
@@ -2740,7 +2743,7 @@
         <v>7113.0806653910067</v>
       </c>
       <c r="G106" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H106" t="s">
         <v>78</v>
@@ -2772,7 +2775,7 @@
         <v>126531.3399274906</v>
       </c>
       <c r="G107" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H107" t="s">
         <v>78</v>
@@ -2804,7 +2807,7 @@
         <v>960.47621643166997</v>
       </c>
       <c r="G108" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H108" t="s">
         <v>78</v>
@@ -2836,7 +2839,7 @@
         <v>126329.45533394575</v>
       </c>
       <c r="G109" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H109" t="s">
         <v>78</v>
@@ -2868,7 +2871,7 @@
         <v>28291.348265977649</v>
       </c>
       <c r="G110" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H110" t="s">
         <v>78</v>
@@ -2900,7 +2903,7 @@
         <v>13223.83785342181</v>
       </c>
       <c r="G111" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H111" t="s">
         <v>78</v>
@@ -2932,7 +2935,7 @@
         <v>4852.7106408946993</v>
       </c>
       <c r="G112" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H112" t="s">
         <v>78</v>
@@ -2964,7 +2967,7 @@
         <v>52626.006382767264</v>
       </c>
       <c r="G113" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H113" t="s">
         <v>78</v>
@@ -2996,7 +2999,7 @@
         <v>505.21348802497369</v>
       </c>
       <c r="G114" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H114" t="s">
         <v>78</v>
@@ -3028,7 +3031,7 @@
         <v>66610.574208923455</v>
       </c>
       <c r="G115" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H115" t="s">
         <v>78</v>
@@ -3060,7 +3063,7 @@
         <v>13917.228747380421</v>
       </c>
       <c r="G116" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H116" t="s">
         <v>78</v>
@@ -3092,7 +3095,7 @@
         <v>7019.2984317250712</v>
       </c>
       <c r="G117" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H117" t="s">
         <v>78</v>
@@ -3124,7 +3127,7 @@
         <v>1005.481013342662</v>
       </c>
       <c r="G118" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H118" t="s">
         <v>78</v>
@@ -3156,7 +3159,7 @@
         <v>18503.403639903867</v>
       </c>
       <c r="G119" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H119" t="s">
         <v>78</v>
@@ -3188,7 +3191,7 @@
         <v>90.462079069437266</v>
       </c>
       <c r="G120" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H120" t="s">
         <v>78</v>
@@ -3220,7 +3223,7 @@
         <v>21792.340945255241</v>
       </c>
       <c r="G121" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H121" t="s">
         <v>78</v>
@@ -3252,7 +3255,7 @@
         <v>4069.5250016077166</v>
       </c>
       <c r="G122" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H122" t="s">
         <v>78</v>
@@ -3284,7 +3287,7 @@
         <v>2243.4524977384435</v>
       </c>
       <c r="G123" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H123" t="s">
         <v>78</v>
@@ -3316,7 +3319,7 @@
         <v>14151.589400801147</v>
       </c>
       <c r="G124" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H124" t="s">
         <v>78</v>
@@ -3348,7 +3351,7 @@
         <v>231888.977058519</v>
       </c>
       <c r="G125" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H125" t="s">
         <v>78</v>
@@ -3380,7 +3383,7 @@
         <v>1935.2646319902863</v>
       </c>
       <c r="G126" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H126" t="s">
         <v>78</v>
@@ -3412,7 +3415,7 @@
         <v>218523.46892550075</v>
       </c>
       <c r="G127" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H127" t="s">
         <v>78</v>
@@ -3444,7 +3447,7 @@
         <v>51329.6267721029</v>
       </c>
       <c r="G128" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H128" t="s">
         <v>78</v>
@@ -3476,7 +3479,7 @@
         <v>23134.354909749345</v>
       </c>
       <c r="G129" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H129" t="s">
         <v>78</v>
@@ -3508,7 +3511,7 @@
         <v>4937.6903790714396</v>
       </c>
       <c r="G130" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H130" t="s">
         <v>78</v>
@@ -3540,7 +3543,7 @@
         <v>66254.468675914773</v>
       </c>
       <c r="G131" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H131" t="s">
         <v>78</v>
@@ -3572,7 +3575,7 @@
         <v>569.48616137572492</v>
       </c>
       <c r="G132" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H132" t="s">
         <v>78</v>
@@ -3604,7 +3607,7 @@
         <v>63428.321923659096</v>
       </c>
       <c r="G133" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H133" t="s">
         <v>78</v>
@@ -3636,7 +3639,7 @@
         <v>14820.10041616484</v>
       </c>
       <c r="G134" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H134" t="s">
         <v>78</v>
@@ -3668,7 +3671,7 @@
         <v>6638.6531875252658</v>
       </c>
       <c r="G135" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H135" t="s">
         <v>78</v>
@@ -3700,7 +3703,7 @@
         <v>8741.8233709328597</v>
       </c>
       <c r="G136" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H136" t="s">
         <v>79</v>
@@ -3732,7 +3735,7 @@
         <v>171449.11775562481</v>
       </c>
       <c r="G137" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H137" t="s">
         <v>79</v>
@@ -3764,7 +3767,7 @@
         <v>1184.3838459816957</v>
       </c>
       <c r="G138" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H138" t="s">
         <v>79</v>
@@ -3796,7 +3799,7 @@
         <v>182370.93078170207</v>
       </c>
       <c r="G139" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H139" t="s">
         <v>79</v>
@@ -3828,7 +3831,7 @@
         <v>39294.847379277948</v>
       </c>
       <c r="G140" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H140" t="s">
         <v>79</v>
@@ -3860,7 +3863,7 @@
         <v>18815.152777425268</v>
       </c>
       <c r="G141" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H141" t="s">
         <v>79</v>
@@ -3892,7 +3895,7 @@
         <v>4982.8384970879915</v>
       </c>
       <c r="G142" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H142" t="s">
         <v>79</v>
@@ -3924,7 +3927,7 @@
         <v>93651.800190535374</v>
       </c>
       <c r="G143" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H143" t="s">
         <v>79</v>
@@ -3956,7 +3959,7 @@
         <v>638.73687074028066</v>
       </c>
       <c r="G144" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H144" t="s">
         <v>79</v>
@@ -3988,7 +3991,7 @@
         <v>96968.471929796026</v>
       </c>
       <c r="G145" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H145" t="s">
         <v>79</v>
@@ -4020,7 +4023,7 @@
         <v>20597.095631125045</v>
       </c>
       <c r="G146" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H146" t="s">
         <v>79</v>
@@ -4052,7 +4055,7 @@
         <v>10094.054249890149</v>
       </c>
       <c r="G147" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H147" t="s">
         <v>79</v>
@@ -4084,7 +4087,7 @@
         <v>12813.561735348043</v>
       </c>
       <c r="G148" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H148" t="s">
         <v>79</v>
@@ -4116,7 +4119,7 @@
         <v>230622.52963454736</v>
       </c>
       <c r="G149" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H149" t="s">
         <v>79</v>
@@ -4148,7 +4151,7 @@
         <v>1720.1413988234976</v>
       </c>
       <c r="G150" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H150" t="s">
         <v>79</v>
@@ -4180,7 +4183,7 @@
         <v>236515.56049280643</v>
       </c>
       <c r="G151" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H151" t="s">
         <v>79</v>
@@ -4212,7 +4215,7 @@
         <v>51184.109413519269</v>
       </c>
       <c r="G152" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H152" t="s">
         <v>79</v>
@@ -4244,7 +4247,7 @@
         <v>24683.485982417478</v>
       </c>
       <c r="G153" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H153" t="s">
         <v>79</v>
@@ -4276,7 +4279,7 @@
         <v>8662.5958500839442</v>
       </c>
       <c r="G154" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H154" t="s">
         <v>79</v>
@@ -4308,7 +4311,7 @@
         <v>150391.81703211847</v>
       </c>
       <c r="G155" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H155" t="s">
         <v>79</v>
@@ -4340,7 +4343,7 @@
         <v>1184.0173440890558</v>
       </c>
       <c r="G156" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H156" t="s">
         <v>79</v>
@@ -4372,7 +4375,7 @@
         <v>153992.18325885473</v>
       </c>
       <c r="G157" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H157" t="s">
         <v>79</v>
@@ -4404,7 +4407,7 @@
         <v>33330.821564507001</v>
       </c>
       <c r="G158" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H158" t="s">
         <v>79</v>
@@ -4436,7 +4439,7 @@
         <v>16017.494274121766</v>
       </c>
       <c r="G159" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H159" t="s">
         <v>79</v>
@@ -4468,7 +4471,7 @@
         <v>4385.4875994898357</v>
       </c>
       <c r="G160" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H160" t="s">
         <v>79</v>
@@ -4500,7 +4503,7 @@
         <v>72183.967579948905</v>
       </c>
       <c r="G161" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H161" t="s">
         <v>79</v>
@@ -4532,7 +4535,7 @@
         <v>552.37615901682693</v>
       </c>
       <c r="G162" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H162" t="s">
         <v>79</v>
@@ -4564,7 +4567,7 @@
         <v>82876.963446566646</v>
       </c>
       <c r="G163" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H163" t="s">
         <v>79</v>
@@ -4596,7 +4599,7 @@
         <v>16633.421923619157</v>
       </c>
       <c r="G164" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H164" t="s">
         <v>79</v>
@@ -4628,7 +4631,7 @@
         <v>8453.4469915325135</v>
       </c>
       <c r="G165" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H165" t="s">
         <v>79</v>
@@ -4660,7 +4663,7 @@
         <v>6316.7706829668077</v>
       </c>
       <c r="G166" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H166" t="s">
         <v>79</v>
@@ -4692,7 +4695,7 @@
         <v>103879.46141404404</v>
       </c>
       <c r="G167" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H167" t="s">
         <v>79</v>
@@ -4724,7 +4727,7 @@
         <v>633.38527389943499</v>
       </c>
       <c r="G168" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H168" t="s">
         <v>79</v>
@@ -4756,7 +4759,7 @@
         <v>111329.05107660916</v>
       </c>
       <c r="G169" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H169" t="s">
         <v>79</v>
@@ -4788,7 +4791,7 @@
         <v>23055.820157082482</v>
       </c>
       <c r="G170" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H170" t="s">
         <v>79</v>
@@ -4820,7 +4823,7 @@
         <v>11338.875358352332</v>
       </c>
       <c r="G171" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H171" t="s">
         <v>79</v>
@@ -4852,7 +4855,7 @@
         <v>11957.455497881961</v>
       </c>
       <c r="G172" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H172" t="s">
         <v>79</v>
@@ -4884,7 +4887,7 @@
         <v>214344.75044877784</v>
       </c>
       <c r="G173" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H173" t="s">
         <v>79</v>
@@ -4916,7 +4919,7 @@
         <v>1638.863971317028</v>
       </c>
       <c r="G174" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H174" t="s">
         <v>79</v>
@@ -4948,7 +4951,7 @@
         <v>211331.51091890014</v>
       </c>
       <c r="G175" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H175" t="s">
         <v>79</v>
@@ -4980,7 +4983,7 @@
         <v>46635.637165848646</v>
       </c>
       <c r="G176" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H176" t="s">
         <v>79</v>
@@ -5012,7 +5015,7 @@
         <v>22120.085478397494</v>
       </c>
       <c r="G177" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H177" t="s">
         <v>79</v>
@@ -5044,7 +5047,7 @@
         <v>9291.2884678487244</v>
       </c>
       <c r="G178" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H178" t="s">
         <v>79</v>
@@ -5076,7 +5079,7 @@
         <v>158419.11006163663</v>
       </c>
       <c r="G179" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H179" t="s">
         <v>79</v>
@@ -5108,7 +5111,7 @@
         <v>1273.1328333784609</v>
       </c>
       <c r="G180" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H180" t="s">
         <v>79</v>
@@ -5140,7 +5143,7 @@
         <v>156036.11502090702</v>
       </c>
       <c r="G181" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H181" t="s">
         <v>79</v>
@@ -5172,7 +5175,7 @@
         <v>34526.176156923604</v>
       </c>
       <c r="G182" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H182" t="s">
         <v>79</v>
@@ -5204,7 +5207,7 @@
         <v>16124.428130304044</v>
       </c>
       <c r="G183" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H183" t="s">
         <v>79</v>
@@ -5236,7 +5239,7 @@
         <v>3922.9156707572961</v>
       </c>
       <c r="G184" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H184" t="s">
         <v>86</v>
@@ -5268,7 +5271,7 @@
         <v>163459.41554513111</v>
       </c>
       <c r="G185" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H185" t="s">
         <v>86</v>
@@ -5300,7 +5303,7 @@
         <v>0</v>
       </c>
       <c r="G186" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H186" t="s">
         <v>86</v>
@@ -5332,7 +5335,7 @@
         <v>297781.30519335077</v>
       </c>
       <c r="G187" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H187" t="s">
         <v>86</v>
@@ -5364,7 +5367,7 @@
         <v>40725.778978910595</v>
       </c>
       <c r="G188" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H188" t="s">
         <v>86</v>
@@ -5396,7 +5399,7 @@
         <v>12945.3532927089</v>
       </c>
       <c r="G189" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H189" t="s">
         <v>86</v>
@@ -5428,7 +5431,7 @@
         <v>7251.1819492944051</v>
       </c>
       <c r="G190" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H190" t="s">
         <v>86</v>
@@ -5460,7 +5463,7 @@
         <v>211701.84854503811</v>
       </c>
       <c r="G191" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H191" t="s">
         <v>86</v>
@@ -5492,7 +5495,7 @@
         <v>0</v>
       </c>
       <c r="G192" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H192" t="s">
         <v>86</v>
@@ -5524,7 +5527,7 @@
         <v>149451.56139251011</v>
       </c>
       <c r="G193" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H193" t="s">
         <v>86</v>
@@ -5556,7 +5559,7 @@
         <v>32904.42057291697</v>
       </c>
       <c r="G194" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H194" t="s">
         <v>86</v>
@@ -5588,7 +5591,7 @@
         <v>19640.218859381792</v>
       </c>
       <c r="G195" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H195" t="s">
         <v>86</v>
@@ -5620,7 +5623,7 @@
         <v>9872.6705855467499</v>
       </c>
       <c r="G196" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H196" t="s">
         <v>86</v>
@@ -5652,7 +5655,7 @@
         <v>89970.55921694405</v>
       </c>
       <c r="G197" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H197" t="s">
         <v>86</v>
@@ -5684,7 +5687,7 @@
         <v>5714.3393546139087</v>
       </c>
       <c r="G198" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H198" t="s">
         <v>86</v>
@@ -5716,7 +5719,7 @@
         <v>165580.93702823977</v>
       </c>
       <c r="G199" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H199" t="s">
         <v>86</v>
@@ -5748,7 +5751,7 @@
         <v>17765.096578689783</v>
       </c>
       <c r="G200" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H200" t="s">
         <v>86</v>
@@ -5780,7 +5783,7 @@
         <v>28696.315640700679</v>
       </c>
       <c r="G201" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H201" t="s">
         <v>86</v>
@@ -5812,7 +5815,7 @@
         <v>11420.06511027717</v>
       </c>
       <c r="G202" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H202" t="s">
         <v>86</v>
@@ -5844,7 +5847,7 @@
         <v>68116.864308526405</v>
       </c>
       <c r="G203" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H203" t="s">
         <v>86</v>
@@ -5876,7 +5879,7 @@
         <v>967.96298444808463</v>
       </c>
       <c r="G204" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H204" t="s">
         <v>86</v>
@@ -5908,7 +5911,7 @@
         <v>49948.285482476509</v>
       </c>
       <c r="G205" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H205" t="s">
         <v>86</v>
@@ -5940,7 +5943,7 @@
         <v>7163.145773291184</v>
       </c>
       <c r="G206" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H206" t="s">
         <v>86</v>
@@ -5972,7 +5975,7 @@
         <v>2352.6572232188714</v>
       </c>
       <c r="G207" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H207" t="s">
         <v>86</v>
@@ -6004,7 +6007,7 @@
         <v>0</v>
       </c>
       <c r="G208" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H208" t="s">
         <v>86</v>
@@ -6036,7 +6039,7 @@
         <v>2775.3252074331208</v>
       </c>
       <c r="G209" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H209" t="s">
         <v>86</v>
@@ -6068,7 +6071,7 @@
         <v>17.530590798671945</v>
       </c>
       <c r="G210" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H210" t="s">
         <v>86</v>
@@ -6100,7 +6103,7 @@
         <v>6503.54405407578</v>
       </c>
       <c r="G211" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H211" t="s">
         <v>86</v>
@@ -6132,7 +6135,7 @@
         <v>540.50570289637517</v>
       </c>
       <c r="G212" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H212" t="s">
         <v>86</v>
@@ -6164,7 +6167,7 @@
         <v>478.83595773052991</v>
       </c>
       <c r="G213" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H213" t="s">
         <v>86</v>
@@ -6196,7 +6199,7 @@
         <v>0</v>
       </c>
       <c r="G214" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H214" t="s">
         <v>86</v>
@@ -6228,7 +6231,7 @@
         <v>10278.088253051208</v>
       </c>
       <c r="G215" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H215" t="s">
         <v>86</v>
@@ -6260,7 +6263,7 @@
         <v>25.751631423550275</v>
       </c>
       <c r="G216" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H216" t="s">
         <v>86</v>
@@ -6292,7 +6295,7 @@
         <v>32773.893960424102</v>
       </c>
       <c r="G217" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H217" t="s">
         <v>86</v>
@@ -6324,7 +6327,7 @@
         <v>2747.8839557221618</v>
       </c>
       <c r="G218" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H218" t="s">
         <v>86</v>
@@ -6356,7 +6359,7 @@
         <v>776.64068644450549</v>
       </c>
       <c r="G219" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H219" t="s">
         <v>86</v>
@@ -6388,7 +6391,7 @@
         <v>3621.2632530121391</v>
       </c>
       <c r="G220" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H220" t="s">
         <v>86</v>
@@ -6420,7 +6423,7 @@
         <v>61930.977722131414</v>
       </c>
       <c r="G221" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H221" t="s">
         <v>86</v>
@@ -6452,7 +6455,7 @@
         <v>1449.1517988260325</v>
       </c>
       <c r="G222" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H222" t="s">
         <v>86</v>
@@ -6484,7 +6487,7 @@
         <v>3217.0997086238362</v>
       </c>
       <c r="G223" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H223" t="s">
         <v>86</v>
@@ -6516,7 +6519,7 @@
         <v>7827.2085275963282</v>
       </c>
       <c r="G224" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H224" t="s">
         <v>86</v>
@@ -6548,7 +6551,7 @@
         <v>4971.7011284687915</v>
       </c>
       <c r="G225" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H225" t="s">
         <v>86</v>
@@ -6580,7 +6583,7 @@
         <v>37217.215401371708</v>
       </c>
       <c r="G226" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H226" t="s">
         <v>86</v>
@@ -6612,7 +6615,7 @@
         <v>97145.531051448546</v>
       </c>
       <c r="G227" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H227" t="s">
         <v>86</v>
@@ -6644,7 +6647,7 @@
         <v>4534.6829452482225</v>
       </c>
       <c r="G228" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H228" t="s">
         <v>86</v>
@@ -6676,7 +6679,7 @@
         <v>14191.095490120413</v>
       </c>
       <c r="G229" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H229" t="s">
         <v>86</v>
@@ -6708,7 +6711,7 @@
         <v>17854.447141101922</v>
       </c>
       <c r="G230" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H230" t="s">
         <v>86</v>
@@ -6740,7 +6743,7 @@
         <v>422.62583205061082</v>
       </c>
       <c r="G231" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H231" t="s">
         <v>86</v>
@@ -6772,7 +6775,7 @@
         <v>3339.2018304202261</v>
       </c>
       <c r="G232" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H232" t="s">
         <v>86</v>
@@ -6804,7 +6807,7 @@
         <v>57344.145387657671</v>
       </c>
       <c r="G233" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H233" t="s">
         <v>86</v>
@@ -6836,7 +6839,7 @@
         <v>502.61895808317564</v>
       </c>
       <c r="G234" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H234" t="s">
         <v>86</v>
@@ -6868,7 +6871,7 @@
         <v>61105.90566759176</v>
       </c>
       <c r="G235" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H235" t="s">
         <v>86</v>
@@ -6900,7 +6903,7 @@
         <v>21668.853295091703</v>
       </c>
       <c r="G236" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H236" t="s">
         <v>86</v>
@@ -6932,7 +6935,7 @@
         <v>2872.2992921317077</v>
       </c>
       <c r="G237" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H237" t="s">
         <v>86</v>
@@ -6964,7 +6967,7 @@
         <v>2708.7083493931427</v>
       </c>
       <c r="G238" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H238" t="s">
         <v>86</v>
@@ -6996,7 +6999,7 @@
         <v>97386.531994692457</v>
       </c>
       <c r="G239" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H239" t="s">
         <v>86</v>
@@ -7028,7 +7031,7 @@
         <v>552.14185157979659</v>
       </c>
       <c r="G240" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H240" t="s">
         <v>86</v>
@@ -7060,7 +7063,7 @@
         <v>43184.299495687977</v>
       </c>
       <c r="G241" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H241" t="s">
         <v>86</v>
@@ -7092,7 +7095,7 @@
         <v>31820.729954511426</v>
       </c>
       <c r="G242" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H242" t="s">
         <v>86</v>
@@ -7124,7 +7127,7 @@
         <v>2618.1555231589746</v>
       </c>
       <c r="G243" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H243" t="s">
         <v>86</v>
@@ -7156,7 +7159,7 @@
         <v>2129.4465859840652</v>
       </c>
       <c r="G244" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H244" t="s">
         <v>86</v>
@@ -7188,7 +7191,7 @@
         <v>9055.2957087368941</v>
       </c>
       <c r="G245" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H245" t="s">
         <v>86</v>
@@ -7220,7 +7223,7 @@
         <v>181.73083811299404</v>
       </c>
       <c r="G246" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H246" t="s">
         <v>86</v>
@@ -7252,7 +7255,7 @@
         <v>2828.4086103025029</v>
       </c>
       <c r="G247" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H247" t="s">
         <v>86</v>
@@ -7284,7 +7287,7 @@
         <v>278.78641360252601</v>
       </c>
       <c r="G248" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H248" t="s">
         <v>86</v>
@@ -7316,7 +7319,7 @@
         <v>450.33271852366653</v>
       </c>
       <c r="G249" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H249" t="s">
         <v>86</v>
@@ -7348,7 +7351,7 @@
         <v>1552.3676342454896</v>
       </c>
       <c r="G250" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H250" t="s">
         <v>86</v>
@@ -7380,7 +7383,7 @@
         <v>7479.9448128556478</v>
       </c>
       <c r="G251" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H251" t="s">
         <v>86</v>
@@ -7412,7 +7415,7 @@
         <v>84.419761887005961</v>
       </c>
       <c r="G252" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H252" t="s">
         <v>86</v>
@@ -7444,7 +7447,7 @@
         <v>3217.9618103574685</v>
       </c>
       <c r="G253" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H253" t="s">
         <v>86</v>
@@ -7476,7 +7479,7 @@
         <v>227.68088345629752</v>
       </c>
       <c r="G254" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H254" t="s">
         <v>86</v>
@@ -7508,7 +7511,7 @@
         <v>841.09559693544384</v>
       </c>
       <c r="G255" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H255" t="s">
         <v>86</v>
@@ -7540,7 +7543,7 @@
         <v>831.82978867327506</v>
       </c>
       <c r="G256" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H256" t="s">
         <v>86</v>
@@ -7572,7 +7575,7 @@
         <v>8379.4092924255619</v>
       </c>
       <c r="G257" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H257" t="s">
         <v>86</v>
@@ -7604,7 +7607,7 @@
         <v>49.821758822385476</v>
       </c>
       <c r="G258" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H258" t="s">
         <v>86</v>
@@ -7636,7 +7639,7 @@
         <v>4675.6603716140271</v>
       </c>
       <c r="G259" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H259" t="s">
         <v>86</v>
@@ -7668,7 +7671,7 @@
         <v>4967.8457685769263</v>
       </c>
       <c r="G260" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H260" t="s">
         <v>86</v>
@@ -7700,7 +7703,7 @@
         <v>448.63676676394709</v>
       </c>
       <c r="G261" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H261" t="s">
         <v>86</v>
@@ -7732,7 +7735,7 @@
         <v>1322.5880632448734</v>
       </c>
       <c r="G262" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H262" t="s">
         <v>86</v>
@@ -7764,7 +7767,7 @@
         <v>10410.181913696766</v>
       </c>
       <c r="G263" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H263" t="s">
         <v>86</v>
@@ -7796,7 +7799,7 @@
         <v>107.39954213459066</v>
       </c>
       <c r="G264" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H264" t="s">
         <v>86</v>
@@ -7828,7 +7831,7 @@
         <v>3753.3815584724898</v>
       </c>
       <c r="G265" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H265" t="s">
         <v>86</v>
@@ -7860,7 +7863,7 @@
         <v>1484.6195744939</v>
       </c>
       <c r="G266" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H266" t="s">
         <v>86</v>
@@ -7892,7 +7895,7 @@
         <v>157.62560108125501</v>
       </c>
       <c r="G267" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H267" t="s">
         <v>86</v>
@@ -7924,7 +7927,7 @@
         <v>15296.15967912087</v>
       </c>
       <c r="G268" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H268" t="s">
         <v>86</v>
@@ -7956,7 +7959,7 @@
         <v>677657.72402788326</v>
       </c>
       <c r="G269" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H269" t="s">
         <v>86</v>
@@ -7988,7 +7991,7 @@
         <v>8721.4201199601648</v>
       </c>
       <c r="G270" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H270" t="s">
         <v>86</v>
@@ -8020,7 +8023,7 @@
         <v>89351.274511664917</v>
       </c>
       <c r="G271" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H271" t="s">
         <v>86</v>
@@ -8052,7 +8055,7 @@
         <v>10247.239765973771</v>
       </c>
       <c r="G272" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H272" t="s">
         <v>86</v>
@@ -8084,7 +8087,7 @@
         <v>6240.657632511703</v>
       </c>
       <c r="G273" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H273" t="s">
         <v>86</v>
@@ -8116,7 +8119,7 @@
         <v>14398.293124016027</v>
       </c>
       <c r="G274" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H274" t="s">
         <v>86</v>
@@ -8148,7 +8151,7 @@
         <v>251356.72111178871</v>
       </c>
       <c r="G275" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H275" t="s">
         <v>86</v>
@@ -8180,7 +8183,7 @@
         <v>4639.3576000601633</v>
       </c>
       <c r="G276" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H276" t="s">
         <v>86</v>
@@ -8212,7 +8215,7 @@
         <v>64338.952803483386</v>
       </c>
       <c r="G277" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H277" t="s">
         <v>86</v>
@@ -8244,7 +8247,7 @@
         <v>24037.762423810709</v>
       </c>
       <c r="G278" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H278" t="s">
         <v>86</v>
@@ -8276,7 +8279,7 @@
         <v>3826.4371997262829</v>
       </c>
       <c r="G279" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H279" t="s">
         <v>86</v>
@@ -8308,7 +8311,7 @@
         <v>4643.1484949014221</v>
       </c>
       <c r="G280" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H280" t="s">
         <v>86</v>
@@ -8340,7 +8343,7 @@
         <v>63887.70220078023</v>
       </c>
       <c r="G281" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H281" t="s">
         <v>86</v>
@@ -8372,7 +8375,7 @@
         <v>1239.2002443851643</v>
       </c>
       <c r="G282" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H282" t="s">
         <v>86</v>
@@ -8404,7 +8407,7 @@
         <v>77806.823939628885</v>
       </c>
       <c r="G283" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H283" t="s">
         <v>86</v>
@@ -8436,7 +8439,7 @@
         <v>30397.652570993756</v>
       </c>
       <c r="G284" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H284" t="s">
         <v>86</v>
@@ -8468,7 +8471,7 @@
         <v>580.30600602523396</v>
       </c>
       <c r="G285" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H285" t="s">
         <v>86</v>
@@ -8500,7 +8503,7 @@
         <v>10211.563068780952</v>
       </c>
       <c r="G286" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H286" t="s">
         <v>86</v>
@@ -8532,7 +8535,7 @@
         <v>184533.24036832617</v>
       </c>
       <c r="G287" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H287" t="s">
         <v>86</v>
@@ -8564,7 +8567,7 @@
         <v>1784.9882158538362</v>
       </c>
       <c r="G288" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H288" t="s">
         <v>86</v>
@@ -8596,7 +8599,7 @@
         <v>142127.91873875455</v>
       </c>
       <c r="G289" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H289" t="s">
         <v>86</v>
@@ -8628,7 +8631,7 @@
         <v>45426.727235972932</v>
       </c>
       <c r="G290" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H290" t="s">
         <v>86</v>
@@ -8660,7 +8663,7 @@
         <v>8258.8755810290222</v>
       </c>
       <c r="G291" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H291" t="s">
         <v>86</v>
@@ -8692,7 +8695,7 @@
         <v>9557.4603031532606</v>
       </c>
       <c r="G292" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H292" t="s">
         <v>86</v>
@@ -8724,7 +8727,7 @@
         <v>145624.29290052608</v>
       </c>
       <c r="G293" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H293" t="s">
         <v>86</v>
@@ -8756,7 +8759,7 @@
         <v>4630.0372042710314</v>
       </c>
       <c r="G294" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H294" t="s">
         <v>86</v>
@@ -8788,7 +8791,7 @@
         <v>219156.55705535915</v>
       </c>
       <c r="G295" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H295" t="s">
         <v>86</v>
@@ -8820,7 +8823,7 @@
         <v>41702.758793559049</v>
       </c>
       <c r="G296" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H296" t="s">
         <v>86</v>
@@ -8852,7 +8855,7 @@
         <v>11752.110271693773</v>
       </c>
       <c r="G297" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H297" t="s">
         <v>86</v>
@@ -8884,7 +8887,7 @@
         <v>9414.942774507088</v>
       </c>
       <c r="G298" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H298" t="s">
         <v>86</v>
@@ -8916,7 +8919,7 @@
         <v>157728.35165002686</v>
       </c>
       <c r="G299" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H299" t="s">
         <v>86</v>
@@ -8948,7 +8951,7 @@
         <v>2608.5796141692022</v>
       </c>
       <c r="G300" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H300" t="s">
         <v>86</v>
@@ -8980,7 +8983,7 @@
         <v>127583.52170839247</v>
       </c>
       <c r="G301" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H301" t="s">
         <v>86</v>
@@ -9012,7 +9015,7 @@
         <v>31197.268389303037</v>
       </c>
       <c r="G302" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H302" t="s">
         <v>86</v>
@@ -9044,7 +9047,7 @@
         <v>19674.119335038991</v>
       </c>
       <c r="G303" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H303" t="s">
         <v>86</v>
@@ -9076,7 +9079,7 @@
         <v>59.937751656536363</v>
       </c>
       <c r="G304" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H304" t="s">
         <v>86</v>
@@ -9108,7 +9111,7 @@
         <v>22570.150663303688</v>
       </c>
       <c r="G305" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H305" t="s">
         <v>86</v>
@@ -9140,7 +9143,7 @@
         <v>12.717102554238107</v>
       </c>
       <c r="G306" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H306" t="s">
         <v>86</v>
@@ -9172,7 +9175,7 @@
         <v>52914.027846697099</v>
       </c>
       <c r="G307" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H307" t="s">
         <v>86</v>
@@ -9204,7 +9207,7 @@
         <v>6167.2112925714964</v>
       </c>
       <c r="G308" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H308" t="s">
         <v>86</v>
@@ -9236,7 +9239,7 @@
         <v>15628.914827420229</v>
       </c>
       <c r="G309" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H309" t="s">
         <v>86</v>
@@ -9268,7 +9271,7 @@
         <v>367.19685618660088</v>
       </c>
       <c r="G310" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H310" t="s">
         <v>86</v>
@@ -9300,7 +9303,7 @@
         <v>33811.061244375509</v>
       </c>
       <c r="G311" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H311" t="s">
         <v>86</v>
@@ -9332,7 +9335,7 @@
         <v>16.694662151644245</v>
       </c>
       <c r="G312" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H312" t="s">
         <v>86</v>
@@ -9364,7 +9367,7 @@
         <v>36023.909835050967</v>
       </c>
       <c r="G313" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H313" t="s">
         <v>86</v>
@@ -9396,7 +9399,7 @@
         <v>9664.2933969973674</v>
       </c>
       <c r="G314" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H314" t="s">
         <v>86</v>
@@ -9428,7 +9431,7 @@
         <v>2136.8845210346039</v>
       </c>
       <c r="G315" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H315" t="s">
         <v>86</v>
@@ -9460,7 +9463,7 @@
         <v>865.02303146035422</v>
       </c>
       <c r="G316" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H316" t="s">
         <v>86</v>
@@ -9492,7 +9495,7 @@
         <v>1322.2321467596173</v>
       </c>
       <c r="G317" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H317" t="s">
         <v>86</v>
@@ -9524,7 +9527,7 @@
         <v>246.76770633396004</v>
       </c>
       <c r="G318" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H318" t="s">
         <v>86</v>
@@ -9556,7 +9559,7 @@
         <v>12516.336862628499</v>
       </c>
       <c r="G319" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H319" t="s">
         <v>86</v>
@@ -9588,7 +9591,7 @@
         <v>650.53286444681021</v>
       </c>
       <c r="G320" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H320" t="s">
         <v>86</v>
@@ -9620,7 +9623,7 @@
         <v>2324.4048202753288</v>
       </c>
       <c r="G321" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H321" t="s">
         <v>86</v>
@@ -9652,7 +9655,7 @@
         <v>344.05955060935412</v>
       </c>
       <c r="G322" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H322" t="s">
         <v>86</v>
@@ -9684,7 +9687,7 @@
         <v>538.72587723692038</v>
       </c>
       <c r="G323" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H323" t="s">
         <v>86</v>
@@ -9716,7 +9719,7 @@
         <v>165.49477391066304</v>
       </c>
       <c r="G324" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H324" t="s">
         <v>86</v>
@@ -9748,7 +9751,7 @@
         <v>10608.7169084712</v>
       </c>
       <c r="G325" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H325" t="s">
         <v>86</v>
@@ -9780,7 +9783,7 @@
         <v>2.9890651801029158</v>
       </c>
       <c r="G326" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H326" t="s">
         <v>86</v>
@@ -9812,7 +9815,7 @@
         <v>861.72059436785958</v>
       </c>
       <c r="G327" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H327" t="s">
         <v>86</v>
@@ -9844,7 +9847,7 @@
         <v>321.63665818847613</v>
       </c>
       <c r="G328" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H328" t="s">
         <v>86</v>
@@ -9876,7 +9879,7 @@
         <v>19571.124797271888</v>
       </c>
       <c r="G329" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H329" t="s">
         <v>86</v>
@@ -9908,7 +9911,7 @@
         <v>17.246000000000002</v>
       </c>
       <c r="G330" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H330" t="s">
         <v>86</v>
@@ -9940,7 +9943,7 @@
         <v>336.61647100528398</v>
       </c>
       <c r="G331" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H331" t="s">
         <v>86</v>
@@ -9972,7 +9975,7 @@
         <v>6479.6878317177006</v>
       </c>
       <c r="G332" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H332" t="s">
         <v>86</v>
@@ -10004,7 +10007,7 @@
         <v>146.732</v>
       </c>
       <c r="G333" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H333" t="s">
         <v>86</v>
@@ -10036,7 +10039,7 @@
         <v>485.18920621830341</v>
       </c>
       <c r="G334" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H334" t="s">
         <v>86</v>
@@ -10068,7 +10071,7 @@
         <v>26771.592829846762</v>
       </c>
       <c r="G335" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H335" t="s">
         <v>86</v>
@@ -10100,7 +10103,7 @@
         <v>188.90300000000002</v>
       </c>
       <c r="G336" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H336" t="s">
         <v>86</v>
@@ -10132,7 +10135,7 @@
         <v>530.36539340149568</v>
       </c>
       <c r="G337" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H337" t="s">
         <v>86</v>
@@ -10164,7 +10167,7 @@
         <v>5778.4188123500962</v>
       </c>
       <c r="G338" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H338" t="s">
         <v>86</v>
@@ -10196,7 +10199,7 @@
         <v>57.486999999999995</v>
       </c>
       <c r="G339" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H339" t="s">
         <v>86</v>
@@ -10228,7 +10231,7 @@
         <v>97.502883519845682</v>
       </c>
       <c r="G340" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H340" t="s">
         <v>86</v>
@@ -10260,7 +10263,7 @@
         <v>49495.205012346581</v>
       </c>
       <c r="G341" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H341" t="s">
         <v>86</v>
@@ -10292,7 +10295,7 @@
         <v>617.07013830971096</v>
       </c>
       <c r="G342" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H342" t="s">
         <v>86</v>
@@ -10324,7 +10327,7 @@
         <v>34675.987504774654</v>
       </c>
       <c r="G343" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H343" t="s">
         <v>86</v>
@@ -10356,7 +10359,7 @@
         <v>6047.1192645228984</v>
       </c>
       <c r="G344" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H344" t="s">
         <v>86</v>
@@ -10388,7 +10391,7 @@
         <v>6347.7556833558338</v>
       </c>
       <c r="G345" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H345" t="s">
         <v>86</v>
@@ -10420,7 +10423,7 @@
         <v>2866.6510499911519</v>
       </c>
       <c r="G346" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H346" t="s">
         <v>86</v>
@@ -10452,7 +10455,7 @@
         <v>21895.422909504425</v>
       </c>
       <c r="G347" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H347" t="s">
         <v>86</v>
@@ -10484,7 +10487,7 @@
         <v>175.69455715983608</v>
       </c>
       <c r="G348" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H348" t="s">
         <v>86</v>
@@ -10516,7 +10519,7 @@
         <v>17629.713549389595</v>
       </c>
       <c r="G349" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H349" t="s">
         <v>86</v>
@@ -10548,7 +10551,7 @@
         <v>1895.9665119371009</v>
       </c>
       <c r="G350" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H350" t="s">
         <v>86</v>
@@ -10580,7 +10583,7 @@
         <v>1226.9109351883744</v>
       </c>
       <c r="G351" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H351" t="s">
         <v>86</v>
@@ -10612,7 +10615,7 @@
         <v>4878.8713759608654</v>
       </c>
       <c r="G352" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H352" t="s">
         <v>86</v>
@@ -10644,7 +10647,7 @@
         <v>21423.228621336257</v>
       </c>
       <c r="G353" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H353" t="s">
         <v>86</v>
@@ -10676,7 +10679,7 @@
         <v>78.661450627454968</v>
       </c>
       <c r="G354" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H354" t="s">
         <v>86</v>
@@ -10708,7 +10711,7 @@
         <v>68630.619154880085</v>
       </c>
       <c r="G355" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H355" t="s">
         <v>86</v>
@@ -10740,7 +10743,7 @@
         <v>30343.273770049575</v>
       </c>
       <c r="G356" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H356" t="s">
         <v>86</v>
@@ -10772,7 +10775,7 @@
         <v>7254.6197592413628</v>
       </c>
       <c r="G357" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H357" t="s">
         <v>86</v>
@@ -10804,7 +10807,7 @@
         <v>4231.1147092942192</v>
       </c>
       <c r="G358" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H358" t="s">
         <v>86</v>
@@ -10836,7 +10839,7 @@
         <v>26779.747408948784</v>
       </c>
       <c r="G359" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H359" t="s">
         <v>86</v>
@@ -10868,7 +10871,7 @@
         <v>38.763634287629955</v>
       </c>
       <c r="G360" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H360" t="s">
         <v>86</v>
@@ -10900,7 +10903,7 @@
         <v>40133.30895769503</v>
       </c>
       <c r="G361" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H361" t="s">
         <v>86</v>
@@ -10932,7 +10935,7 @@
         <v>3183.0024543966538</v>
       </c>
       <c r="G362" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H362" t="s">
         <v>86</v>
@@ -10964,7 +10967,7 @@
         <v>954.51285213324832</v>
       </c>
       <c r="G363" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H363" t="s">
         <v>86</v>
@@ -10996,7 +10999,7 @@
         <v>796.38982757352926</v>
       </c>
       <c r="G364" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H364" t="s">
         <v>86</v>
@@ -11028,7 +11031,7 @@
         <v>14523.278234305888</v>
       </c>
       <c r="G365" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H365" t="s">
         <v>86</v>
@@ -11060,7 +11063,7 @@
         <v>295.03658045309834</v>
       </c>
       <c r="G366" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H366" t="s">
         <v>86</v>
@@ -11092,7 +11095,7 @@
         <v>29747.905867875084</v>
       </c>
       <c r="G367" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H367" t="s">
         <v>86</v>
@@ -11124,7 +11127,7 @@
         <v>5869.6727564367684</v>
       </c>
       <c r="G368" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H368" t="s">
         <v>86</v>
@@ -11156,7 +11159,7 @@
         <v>7403.5774247271083</v>
       </c>
       <c r="G369" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H369" t="s">
         <v>86</v>
@@ -11188,7 +11191,7 @@
         <v>752.4861724264706</v>
       </c>
       <c r="G370" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H370" t="s">
         <v>86</v>
@@ -11220,7 +11223,7 @@
         <v>28885.040765694099</v>
       </c>
       <c r="G371" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H371" t="s">
         <v>86</v>
@@ -11252,7 +11255,7 @@
         <v>255.76941954690156</v>
       </c>
       <c r="G372" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H372" t="s">
         <v>86</v>
@@ -11284,7 +11287,7 @@
         <v>20064.459132124935</v>
       </c>
       <c r="G373" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H373" t="s">
         <v>86</v>
@@ -11316,7 +11319,7 @@
         <v>5438.168243563232</v>
       </c>
       <c r="G374" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H374" t="s">
         <v>86</v>
@@ -11348,7 +11351,7 @@
         <v>515.28357527289188</v>
       </c>
       <c r="G375" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H375" t="s">
         <v>86</v>
@@ -21457,8 +21460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A94BF84-AB01-45F2-8A1E-DD5B502642C6}">
   <dimension ref="A1:Q117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P96" sqref="P96"/>
+    <sheetView topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U104" sqref="U104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21527,7 +21530,7 @@
         <v>36</v>
       </c>
       <c r="N2" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -21541,7 +21544,7 @@
         <v>36</v>
       </c>
       <c r="N3" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -21555,7 +21558,7 @@
         <v>36</v>
       </c>
       <c r="N4" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -21569,7 +21572,7 @@
         <v>36</v>
       </c>
       <c r="N5" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -21583,7 +21586,7 @@
         <v>36</v>
       </c>
       <c r="N6" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -21597,7 +21600,7 @@
         <v>36</v>
       </c>
       <c r="N7" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -21611,7 +21614,7 @@
         <v>36</v>
       </c>
       <c r="N8" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -21625,7 +21628,7 @@
         <v>36</v>
       </c>
       <c r="N9" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -21642,7 +21645,7 @@
         <v>36</v>
       </c>
       <c r="N10" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="O10" t="s">
         <v>78</v>
@@ -21665,7 +21668,7 @@
         <v>36</v>
       </c>
       <c r="N11" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="O11" t="s">
         <v>78</v>
@@ -21688,7 +21691,7 @@
         <v>36</v>
       </c>
       <c r="N12" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="O12" t="s">
         <v>78</v>
@@ -21708,7 +21711,7 @@
         <v>36</v>
       </c>
       <c r="N13" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -21725,7 +21728,7 @@
         <v>36</v>
       </c>
       <c r="N14" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="O14" t="s">
         <v>78</v>
@@ -21748,7 +21751,7 @@
         <v>36</v>
       </c>
       <c r="N15" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="O15" t="s">
         <v>78</v>
@@ -21771,7 +21774,7 @@
         <v>36</v>
       </c>
       <c r="N16" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="O16" t="s">
         <v>78</v>
@@ -21794,7 +21797,7 @@
         <v>36</v>
       </c>
       <c r="N17" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="O17" t="s">
         <v>78</v>
@@ -21817,7 +21820,7 @@
         <v>36</v>
       </c>
       <c r="N18" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="O18" t="s">
         <v>78</v>
@@ -21837,7 +21840,7 @@
         <v>36</v>
       </c>
       <c r="N19" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -21851,7 +21854,7 @@
         <v>36</v>
       </c>
       <c r="N20" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
@@ -21865,7 +21868,7 @@
         <v>36</v>
       </c>
       <c r="N21" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -21879,7 +21882,7 @@
         <v>36</v>
       </c>
       <c r="N22" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
@@ -23987,7 +23990,7 @@
         <v>38</v>
       </c>
       <c r="N86" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="O86" t="s">
         <v>86</v>
@@ -24040,7 +24043,7 @@
         <v>38</v>
       </c>
       <c r="N87" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="O87" t="s">
         <v>86</v>
@@ -24093,7 +24096,7 @@
         <v>38</v>
       </c>
       <c r="N88" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="O88" t="s">
         <v>86</v>
@@ -24146,7 +24149,7 @@
         <v>38</v>
       </c>
       <c r="N89" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="O89" t="s">
         <v>86</v>
@@ -24175,7 +24178,7 @@
         <v>38</v>
       </c>
       <c r="N90" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="O90" t="s">
         <v>86</v>
@@ -24201,7 +24204,7 @@
         <v>38</v>
       </c>
       <c r="N91" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="O91" t="s">
         <v>86</v>
@@ -24227,7 +24230,7 @@
         <v>38</v>
       </c>
       <c r="N92" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="O92" t="s">
         <v>86</v>
@@ -24253,7 +24256,7 @@
         <v>38</v>
       </c>
       <c r="N93" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="O93" t="s">
         <v>86</v>
@@ -34625,6 +34628,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000614419EC33FAD42A0282CFF32600A20" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="699fc316e813a14ea4ed1705cd009a31">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d4f3f700-51b4-43ff-b002-6ed848604d46" xmlns:ns3="01f01bef-47b7-4725-adaf-9b6a8bd74ef4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60f45b07400bba80031d5d187855d3df" ns2:_="" ns3:_="">
     <xsd:import namespace="d4f3f700-51b4-43ff-b002-6ed848604d46"/>
@@ -34827,15 +34839,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22AD2C85-521D-4770-88CD-9DAE105CB1B6}">
   <ds:schemaRefs>
@@ -34846,6 +34849,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{729962EC-F35D-459B-8881-4F6AA84AC69F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06F29519-FBA5-4771-9A2F-A4B6B88124FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -34862,12 +34873,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{729962EC-F35D-459B-8881-4F6AA84AC69F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update Hucuktlis age samples
</commit_message>
<xml_diff>
--- a/1. data/Barkley Sockeye time series of returns.xlsx
+++ b/1. data/Barkley Sockeye time series of returns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://086gc.sharepoint.com/sites/SalmonScienceStrategy-salmonFSAR/Shared Documents/salmon FSAR - sprint week/Barkley Sockeye/3. Data/Stock-recruit data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="758" documentId="13_ncr:1_{3A0DAE0A-5A1E-485E-89C6-BA3AF7C7CFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2EF2ED4-E85B-4F51-8ED5-A839A73EFB37}"/>
+  <xr:revisionPtr revIDLastSave="879" documentId="13_ncr:1_{3A0DAE0A-5A1E-485E-89C6-BA3AF7C7CFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F26EC160-20AE-4E07-91DB-04BA3B87CF17}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data sources notes" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Age_samples" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Hucuktlis!$A$1:$O$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Hucuktlis!$A$1:$O$123</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Somass!$A$1:$I$663</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5041" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5072" uniqueCount="117">
   <si>
     <t>GCL</t>
   </si>
@@ -403,9 +403,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -474,7 +475,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -482,6 +483,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1049,7 +1051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J663"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H667" sqref="H667"/>
     </sheetView>
@@ -21458,10 +21460,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A94BF84-AB01-45F2-8A1E-DD5B502642C6}">
-  <dimension ref="A1:Q117"/>
+  <dimension ref="A1:Q123"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U104" sqref="U104"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I125" sqref="I125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24122,28 +24125,28 @@
         <v>20</v>
       </c>
       <c r="E89">
-        <v>137</v>
-      </c>
-      <c r="F89">
-        <v>0</v>
-      </c>
-      <c r="G89">
-        <v>0.29702970297029702</v>
-      </c>
-      <c r="H89">
-        <v>0.60396039603960394</v>
-      </c>
-      <c r="I89">
-        <v>0</v>
-      </c>
-      <c r="J89">
-        <v>0</v>
-      </c>
-      <c r="K89">
-        <v>9.9009900990099011E-3</v>
-      </c>
-      <c r="L89">
-        <v>8.9108910891089105E-2</v>
+        <v>152</v>
+      </c>
+      <c r="F89" s="5">
+        <v>0</v>
+      </c>
+      <c r="G89" s="5">
+        <v>0.30263157889999998</v>
+      </c>
+      <c r="H89" s="5">
+        <v>0.60526315789999996</v>
+      </c>
+      <c r="I89" s="5">
+        <v>0</v>
+      </c>
+      <c r="J89" s="5">
+        <v>0</v>
+      </c>
+      <c r="K89" s="5">
+        <v>6.5789474000000001E-3</v>
+      </c>
+      <c r="L89" s="5">
+        <v>8.5526315800000002E-2</v>
       </c>
       <c r="M89" t="s">
         <v>38</v>
@@ -24171,7 +24174,31 @@
       <c r="C90">
         <v>237</v>
       </c>
+      <c r="D90" t="s">
+        <v>42</v>
+      </c>
       <c r="E90">
+        <v>109</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>0.42202000000000001</v>
+      </c>
+      <c r="H90">
+        <v>0.27522999999999997</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <v>0.30275000000000002</v>
+      </c>
+      <c r="L90">
         <v>0</v>
       </c>
       <c r="M90" t="s">
@@ -24852,28 +24879,30 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B106">
-        <v>6400</v>
+        <v>11837</v>
       </c>
       <c r="C106">
-        <v>5192</v>
+        <v>21656</v>
       </c>
       <c r="D106" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E106">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="F106">
         <v>0</v>
       </c>
       <c r="G106">
-        <v>1</v>
+        <f>4/E106</f>
+        <v>0.12121212121212122</v>
       </c>
       <c r="H106">
-        <v>0</v>
+        <f>28/E106</f>
+        <v>0.84848484848484851</v>
       </c>
       <c r="I106">
         <v>0</v>
@@ -24882,7 +24911,8 @@
         <v>0</v>
       </c>
       <c r="K106">
-        <v>0</v>
+        <f>1/E106</f>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="L106">
         <v>0</v>
@@ -24902,28 +24932,28 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B107">
-        <v>10700</v>
+        <v>6400</v>
       </c>
       <c r="C107">
-        <v>23111</v>
+        <v>5192</v>
       </c>
       <c r="D107" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E107">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="F107">
         <v>0</v>
       </c>
       <c r="G107">
-        <v>7.0000000000000007E-2</v>
+        <v>1</v>
       </c>
       <c r="H107">
-        <v>0.93</v>
+        <v>0</v>
       </c>
       <c r="I107">
         <v>0</v>
@@ -24952,28 +24982,28 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B108">
-        <v>10700</v>
+        <v>6400</v>
       </c>
       <c r="C108">
-        <v>23111</v>
+        <v>5192</v>
       </c>
       <c r="D108" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E108">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="F108">
         <v>0</v>
       </c>
       <c r="G108">
-        <v>6.9306930693069313E-2</v>
+        <v>1</v>
       </c>
       <c r="H108">
-        <v>0.91089108910891092</v>
+        <v>0</v>
       </c>
       <c r="I108">
         <v>0</v>
@@ -24982,7 +25012,7 @@
         <v>0</v>
       </c>
       <c r="K108">
-        <v>1.9801980198019802E-2</v>
+        <v>0</v>
       </c>
       <c r="L108">
         <v>0</v>
@@ -25002,31 +25032,31 @@
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B109">
-        <v>22704</v>
+        <v>10700</v>
       </c>
       <c r="C109">
-        <v>3217</v>
+        <v>23111</v>
       </c>
       <c r="D109" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E109">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="F109">
         <v>0</v>
       </c>
       <c r="G109">
-        <v>0.59</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H109">
-        <v>0.36</v>
+        <v>0.93</v>
       </c>
       <c r="I109">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="J109">
         <v>0</v>
@@ -25052,28 +25082,28 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B110">
-        <v>12203</v>
+        <v>10700</v>
       </c>
       <c r="C110">
-        <v>626</v>
+        <v>23111</v>
       </c>
       <c r="D110" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E110">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="F110">
         <v>0</v>
       </c>
       <c r="G110">
-        <v>0.11</v>
+        <v>6.9306930693069313E-2</v>
       </c>
       <c r="H110">
-        <v>0.89</v>
+        <v>0.91089108910891092</v>
       </c>
       <c r="I110">
         <v>0</v>
@@ -25082,7 +25112,7 @@
         <v>0</v>
       </c>
       <c r="K110">
-        <v>0</v>
+        <v>1.9801980198019802E-2</v>
       </c>
       <c r="L110">
         <v>0</v>
@@ -25102,31 +25132,31 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="B111">
-        <v>13549</v>
+        <v>22704</v>
       </c>
       <c r="C111">
-        <v>154</v>
+        <v>3217</v>
       </c>
       <c r="D111" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E111">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="F111">
         <v>0</v>
       </c>
       <c r="G111">
-        <v>0</v>
+        <v>0.59</v>
       </c>
       <c r="H111">
-        <v>1</v>
+        <v>0.36</v>
       </c>
       <c r="I111">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J111">
         <v>0</v>
@@ -25152,18 +25182,41 @@
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="B112">
-        <v>4589</v>
+        <v>22704</v>
       </c>
       <c r="C112">
-        <v>443</v>
+        <v>3217</v>
       </c>
       <c r="D112" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E112">
+        <v>28</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112">
+        <f>20/E112</f>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="H112">
+        <f>8/E112</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="I112">
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>0</v>
+      </c>
+      <c r="K112">
+        <v>0</v>
+      </c>
+      <c r="L112">
         <v>0</v>
       </c>
       <c r="N112" t="s">
@@ -25181,28 +25234,28 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="B113">
-        <v>14520</v>
+        <v>12203</v>
       </c>
       <c r="C113">
-        <v>4359</v>
+        <v>626</v>
       </c>
       <c r="D113" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E113">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="F113">
         <v>0</v>
       </c>
       <c r="G113">
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="I113">
         <v>0</v>
@@ -25231,28 +25284,30 @@
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="B114">
-        <v>18646</v>
+        <v>12203</v>
       </c>
       <c r="C114">
-        <v>7731</v>
+        <v>626</v>
       </c>
       <c r="D114" t="s">
         <v>34</v>
       </c>
       <c r="E114">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="F114">
         <v>0</v>
       </c>
       <c r="G114">
-        <v>0.35820895522388058</v>
+        <f>11/E114</f>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H114">
-        <v>0.62686567164179108</v>
+        <f>22/E114</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I114">
         <v>0</v>
@@ -25264,7 +25319,7 @@
         <v>0</v>
       </c>
       <c r="L114">
-        <v>1.4925373134328358E-2</v>
+        <v>0</v>
       </c>
       <c r="N114" t="s">
         <v>44</v>
@@ -25281,28 +25336,28 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="B115">
-        <v>18646</v>
+        <v>13549</v>
       </c>
       <c r="C115">
-        <v>7731</v>
+        <v>154</v>
       </c>
       <c r="D115" t="s">
         <v>32</v>
       </c>
       <c r="E115">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F115">
         <v>0</v>
       </c>
       <c r="G115">
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="H115">
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="I115">
         <v>0</v>
@@ -25331,28 +25386,28 @@
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="B116">
-        <v>13113</v>
+        <v>13549</v>
       </c>
       <c r="C116">
-        <v>8196</v>
+        <v>154</v>
       </c>
       <c r="D116" t="s">
         <v>34</v>
       </c>
       <c r="E116">
-        <v>151</v>
+        <v>5</v>
       </c>
       <c r="F116">
         <v>0</v>
       </c>
       <c r="G116">
-        <v>0.19867549668874171</v>
+        <v>0</v>
       </c>
       <c r="H116">
-        <v>0.7814569536423841</v>
+        <v>1</v>
       </c>
       <c r="I116">
         <v>0</v>
@@ -25361,10 +25416,10 @@
         <v>0</v>
       </c>
       <c r="K116">
-        <v>6.6225165562913907E-3</v>
+        <v>0</v>
       </c>
       <c r="L116">
-        <v>1.3245033112582781E-2</v>
+        <v>0</v>
       </c>
       <c r="N116" t="s">
         <v>44</v>
@@ -25381,31 +25436,34 @@
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="B117">
-        <v>13113</v>
+        <v>4589</v>
       </c>
       <c r="C117">
-        <v>8196</v>
+        <v>443</v>
       </c>
       <c r="D117" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E117">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F117">
         <v>0</v>
       </c>
       <c r="G117">
-        <v>0.14285714285714285</v>
+        <f>7/E117</f>
+        <v>0.7</v>
       </c>
       <c r="H117">
-        <v>0.8571428571428571</v>
+        <f>2/E117</f>
+        <v>0.2</v>
       </c>
       <c r="I117">
-        <v>0</v>
+        <f>1/E117</f>
+        <v>0.1</v>
       </c>
       <c r="J117">
         <v>0</v>
@@ -25426,6 +25484,310 @@
         <v>41</v>
       </c>
       <c r="Q117" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>2021</v>
+      </c>
+      <c r="B118">
+        <v>14520</v>
+      </c>
+      <c r="C118">
+        <v>4359</v>
+      </c>
+      <c r="D118" t="s">
+        <v>33</v>
+      </c>
+      <c r="E118">
+        <v>7</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+      <c r="G118">
+        <v>1</v>
+      </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
+      <c r="I118">
+        <v>0</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
+      </c>
+      <c r="K118">
+        <v>0</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
+      </c>
+      <c r="N118" t="s">
+        <v>44</v>
+      </c>
+      <c r="O118" t="s">
+        <v>86</v>
+      </c>
+      <c r="P118" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q118" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>2021</v>
+      </c>
+      <c r="B119">
+        <v>14520</v>
+      </c>
+      <c r="C119">
+        <v>4359</v>
+      </c>
+      <c r="D119" t="s">
+        <v>34</v>
+      </c>
+      <c r="E119">
+        <v>155</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+      <c r="G119">
+        <f>129/E119</f>
+        <v>0.83225806451612905</v>
+      </c>
+      <c r="H119">
+        <f>23/E119</f>
+        <v>0.14838709677419354</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+      <c r="K119">
+        <f>1/E119</f>
+        <v>6.4516129032258064E-3</v>
+      </c>
+      <c r="L119">
+        <f>2/E119</f>
+        <v>1.2903225806451613E-2</v>
+      </c>
+      <c r="N119" t="s">
+        <v>44</v>
+      </c>
+      <c r="O119" t="s">
+        <v>86</v>
+      </c>
+      <c r="P119" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>2022</v>
+      </c>
+      <c r="B120">
+        <v>18646</v>
+      </c>
+      <c r="C120">
+        <v>7731</v>
+      </c>
+      <c r="D120" t="s">
+        <v>34</v>
+      </c>
+      <c r="E120">
+        <v>67</v>
+      </c>
+      <c r="F120">
+        <v>0</v>
+      </c>
+      <c r="G120">
+        <v>0.35820895522388058</v>
+      </c>
+      <c r="H120">
+        <v>0.62686567164179108</v>
+      </c>
+      <c r="I120">
+        <v>0</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120">
+        <v>0</v>
+      </c>
+      <c r="L120">
+        <v>1.4925373134328358E-2</v>
+      </c>
+      <c r="N120" t="s">
+        <v>44</v>
+      </c>
+      <c r="O120" t="s">
+        <v>86</v>
+      </c>
+      <c r="P120" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>2022</v>
+      </c>
+      <c r="B121">
+        <v>18646</v>
+      </c>
+      <c r="C121">
+        <v>7731</v>
+      </c>
+      <c r="D121" t="s">
+        <v>32</v>
+      </c>
+      <c r="E121">
+        <v>15</v>
+      </c>
+      <c r="F121">
+        <v>0</v>
+      </c>
+      <c r="G121">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H121">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I121">
+        <v>0</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
+      <c r="K121">
+        <v>0</v>
+      </c>
+      <c r="L121">
+        <v>0</v>
+      </c>
+      <c r="N121" t="s">
+        <v>44</v>
+      </c>
+      <c r="O121" t="s">
+        <v>86</v>
+      </c>
+      <c r="P121" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>2023</v>
+      </c>
+      <c r="B122">
+        <v>13113</v>
+      </c>
+      <c r="C122">
+        <v>8196</v>
+      </c>
+      <c r="D122" t="s">
+        <v>34</v>
+      </c>
+      <c r="E122">
+        <v>151</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+      <c r="G122">
+        <v>0.19867549668874171</v>
+      </c>
+      <c r="H122">
+        <v>0.7814569536423841</v>
+      </c>
+      <c r="I122">
+        <v>0</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+      <c r="K122">
+        <v>6.6225165562913907E-3</v>
+      </c>
+      <c r="L122">
+        <v>1.3245033112582781E-2</v>
+      </c>
+      <c r="N122" t="s">
+        <v>44</v>
+      </c>
+      <c r="O122" t="s">
+        <v>86</v>
+      </c>
+      <c r="P122" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>2023</v>
+      </c>
+      <c r="B123">
+        <v>13113</v>
+      </c>
+      <c r="C123">
+        <v>8196</v>
+      </c>
+      <c r="D123" t="s">
+        <v>32</v>
+      </c>
+      <c r="E123">
+        <v>7</v>
+      </c>
+      <c r="F123">
+        <v>0</v>
+      </c>
+      <c r="G123">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="H123">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="J123">
+        <v>0</v>
+      </c>
+      <c r="K123">
+        <v>0</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+      <c r="N123" t="s">
+        <v>44</v>
+      </c>
+      <c r="O123" t="s">
+        <v>86</v>
+      </c>
+      <c r="P123" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q123" t="s">
         <v>39</v>
       </c>
     </row>
@@ -25439,7 +25801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FC0BAD-3412-4CD1-924D-26A01469586A}">
   <dimension ref="A1:F277"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A280" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -29853,8 +30215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{116A4842-63E3-4614-A73E-CB32DDB2B86D}">
   <dimension ref="A1:G245"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="F275" sqref="F275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33938,7 +34300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F161B800-98B7-4043-8D52-286424C777BB}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix small data entry error for Hucuktlis 2001 escapement data source
</commit_message>
<xml_diff>
--- a/1. data/Barkley Sockeye time series of returns.xlsx
+++ b/1. data/Barkley Sockeye time series of returns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://086gc.sharepoint.com/sites/SalmonScienceStrategy-salmonFSAR/Shared Documents/salmon FSAR - sprint week/Barkley Sockeye/3. Data/Stock-recruit data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1248" documentId="13_ncr:1_{3A0DAE0A-5A1E-485E-89C6-BA3AF7C7CFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE463298-458B-46AB-B3FC-7A8F2913DC1C}"/>
+  <xr:revisionPtr revIDLastSave="1250" documentId="13_ncr:1_{3A0DAE0A-5A1E-485E-89C6-BA3AF7C7CFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5F06693-F4CA-43C2-AF6A-E335E9115B6E}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data sources notes" sheetId="5" r:id="rId1"/>
@@ -25719,12 +25719,13 @@
   <dimension ref="A1:T126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q92" sqref="Q92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -29127,7 +29128,7 @@
         <v>38</v>
       </c>
       <c r="Q91" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="R91" t="s">
         <v>86</v>
@@ -40945,15 +40946,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000614419EC33FAD42A0282CFF32600A20" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b94ec4c5b022f3c1dd5ef88a1c70be4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d4f3f700-51b4-43ff-b002-6ed848604d46" xmlns:ns3="01f01bef-47b7-4725-adaf-9b6a8bd74ef4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0d993d6f0fe140b5b27b8bdb1a11ff43" ns2:_="" ns3:_="">
     <xsd:import namespace="d4f3f700-51b4-43ff-b002-6ed848604d46"/>
@@ -41162,6 +41154,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22AD2C85-521D-4770-88CD-9DAE105CB1B6}">
   <ds:schemaRefs>
@@ -41172,14 +41173,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{729962EC-F35D-459B-8881-4F6AA84AC69F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83F8A5F1-9F5C-410C-A02F-9F6149407001}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41196,4 +41189,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{729962EC-F35D-459B-8881-4F6AA84AC69F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add 2024 run reconstruction data
</commit_message>
<xml_diff>
--- a/1. data/Barkley Sockeye time series of returns.xlsx
+++ b/1. data/Barkley Sockeye time series of returns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://086gc.sharepoint.com/sites/SalmonScienceStrategy-salmonFSAR/Shared Documents/salmon FSAR - sprint week/Barkley Sockeye/3. Data/Stock-recruit data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\Barkley-Sk-CSAS\1. data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1250" documentId="13_ncr:1_{3A0DAE0A-5A1E-485E-89C6-BA3AF7C7CFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5F06693-F4CA-43C2-AF6A-E335E9115B6E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E5154F-BC5F-4A6C-9F3D-16808F8FD8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data sources notes" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5112" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5177" uniqueCount="138">
   <si>
     <t>GCL</t>
   </si>
@@ -1124,9 +1124,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L677"/>
+  <dimension ref="A1:L689"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
@@ -1184,6 +1184,9 @@
       <c r="B2">
         <v>1921</v>
       </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
       <c r="H2">
         <f>1344000+112000+448000+336000+448000</f>
         <v>2688000</v>
@@ -1196,6 +1199,9 @@
       <c r="B3">
         <v>1921</v>
       </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
       <c r="H3">
         <f>80000+112000+1120000</f>
         <v>1312000</v>
@@ -24834,6 +24840,462 @@
         <v>39</v>
       </c>
       <c r="L677" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="678" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A678" t="s">
+        <v>0</v>
+      </c>
+      <c r="B678">
+        <v>2024</v>
+      </c>
+      <c r="C678" s="1">
+        <v>3</v>
+      </c>
+      <c r="D678" s="1">
+        <v>2</v>
+      </c>
+      <c r="E678">
+        <v>44034.592196495687</v>
+      </c>
+      <c r="F678">
+        <v>1833.3676334248605</v>
+      </c>
+      <c r="G678">
+        <v>1</v>
+      </c>
+      <c r="H678">
+        <v>0</v>
+      </c>
+      <c r="I678" t="s">
+        <v>57</v>
+      </c>
+      <c r="J678" t="s">
+        <v>86</v>
+      </c>
+      <c r="K678" t="s">
+        <v>39</v>
+      </c>
+      <c r="L678" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="679" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A679" t="s">
+        <v>0</v>
+      </c>
+      <c r="B679">
+        <v>2024</v>
+      </c>
+      <c r="C679" s="1">
+        <v>4</v>
+      </c>
+      <c r="D679" s="1">
+        <v>2</v>
+      </c>
+      <c r="E679">
+        <v>268331.71659599483</v>
+      </c>
+      <c r="F679">
+        <v>159033.37039591704</v>
+      </c>
+      <c r="G679">
+        <v>1</v>
+      </c>
+      <c r="H679">
+        <v>0</v>
+      </c>
+      <c r="I679" t="s">
+        <v>57</v>
+      </c>
+      <c r="J679" t="s">
+        <v>86</v>
+      </c>
+      <c r="K679" t="s">
+        <v>39</v>
+      </c>
+      <c r="L679" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="680" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A680" t="s">
+        <v>0</v>
+      </c>
+      <c r="B680">
+        <v>2024</v>
+      </c>
+      <c r="C680" s="1">
+        <v>4</v>
+      </c>
+      <c r="D680" s="1">
+        <v>3</v>
+      </c>
+      <c r="E680">
+        <v>5652.1760715499395</v>
+      </c>
+      <c r="F680">
+        <v>820.23780905801345</v>
+      </c>
+      <c r="G680">
+        <v>1</v>
+      </c>
+      <c r="H680">
+        <v>0</v>
+      </c>
+      <c r="I680" t="s">
+        <v>57</v>
+      </c>
+      <c r="J680" t="s">
+        <v>86</v>
+      </c>
+      <c r="K680" t="s">
+        <v>39</v>
+      </c>
+      <c r="L680" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="681" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A681" t="s">
+        <v>0</v>
+      </c>
+      <c r="B681">
+        <v>2024</v>
+      </c>
+      <c r="C681" s="1">
+        <v>5</v>
+      </c>
+      <c r="D681" s="1">
+        <v>2</v>
+      </c>
+      <c r="E681">
+        <v>38399.017398105898</v>
+      </c>
+      <c r="F681">
+        <v>39429.947858773899</v>
+      </c>
+      <c r="G681">
+        <v>1</v>
+      </c>
+      <c r="H681">
+        <v>0</v>
+      </c>
+      <c r="I681" t="s">
+        <v>57</v>
+      </c>
+      <c r="J681" t="s">
+        <v>86</v>
+      </c>
+      <c r="K681" t="s">
+        <v>39</v>
+      </c>
+      <c r="L681" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="682" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A682" t="s">
+        <v>0</v>
+      </c>
+      <c r="B682">
+        <v>2024</v>
+      </c>
+      <c r="C682" s="1">
+        <v>5</v>
+      </c>
+      <c r="D682" s="1">
+        <v>3</v>
+      </c>
+      <c r="E682">
+        <v>14554.771097609648</v>
+      </c>
+      <c r="F682">
+        <v>7208.322237147273</v>
+      </c>
+      <c r="G682">
+        <v>1</v>
+      </c>
+      <c r="H682">
+        <v>0</v>
+      </c>
+      <c r="I682" t="s">
+        <v>57</v>
+      </c>
+      <c r="J682" t="s">
+        <v>86</v>
+      </c>
+      <c r="K682" t="s">
+        <v>39</v>
+      </c>
+      <c r="L682" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="683" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A683" t="s">
+        <v>0</v>
+      </c>
+      <c r="B683">
+        <v>2024</v>
+      </c>
+      <c r="C683" s="1">
+        <v>6</v>
+      </c>
+      <c r="D683" s="1">
+        <v>3</v>
+      </c>
+      <c r="E683">
+        <v>2686.7266402438008</v>
+      </c>
+      <c r="F683">
+        <v>3352.8454258667534</v>
+      </c>
+      <c r="G683">
+        <v>1</v>
+      </c>
+      <c r="H683">
+        <v>0</v>
+      </c>
+      <c r="I683" t="s">
+        <v>57</v>
+      </c>
+      <c r="J683" t="s">
+        <v>86</v>
+      </c>
+      <c r="K683" t="s">
+        <v>39</v>
+      </c>
+      <c r="L683" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="684" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A684" t="s">
+        <v>1</v>
+      </c>
+      <c r="B684">
+        <v>2024</v>
+      </c>
+      <c r="C684" s="1">
+        <v>3</v>
+      </c>
+      <c r="D684" s="1">
+        <v>2</v>
+      </c>
+      <c r="E684">
+        <v>39735.777080015832</v>
+      </c>
+      <c r="F684">
+        <v>3826.1618478795608</v>
+      </c>
+      <c r="G684">
+        <v>0</v>
+      </c>
+      <c r="H684">
+        <v>0</v>
+      </c>
+      <c r="I684" t="s">
+        <v>57</v>
+      </c>
+      <c r="J684" t="s">
+        <v>86</v>
+      </c>
+      <c r="K684" t="s">
+        <v>39</v>
+      </c>
+      <c r="L684" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="685" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A685" t="s">
+        <v>1</v>
+      </c>
+      <c r="B685">
+        <v>2024</v>
+      </c>
+      <c r="C685" s="1">
+        <v>4</v>
+      </c>
+      <c r="D685" s="1">
+        <v>2</v>
+      </c>
+      <c r="E685">
+        <v>61909.641764322092</v>
+      </c>
+      <c r="F685">
+        <v>50613.402972045842</v>
+      </c>
+      <c r="G685">
+        <v>0</v>
+      </c>
+      <c r="H685">
+        <v>0</v>
+      </c>
+      <c r="I685" t="s">
+        <v>57</v>
+      </c>
+      <c r="J685" t="s">
+        <v>86</v>
+      </c>
+      <c r="K685" t="s">
+        <v>39</v>
+      </c>
+      <c r="L685" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="686" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A686" t="s">
+        <v>1</v>
+      </c>
+      <c r="B686">
+        <v>2024</v>
+      </c>
+      <c r="C686" s="1">
+        <v>4</v>
+      </c>
+      <c r="D686" s="1">
+        <v>3</v>
+      </c>
+      <c r="E686">
+        <v>2386.7921965356168</v>
+      </c>
+      <c r="F686">
+        <v>378.60972498212408</v>
+      </c>
+      <c r="G686">
+        <v>0</v>
+      </c>
+      <c r="H686">
+        <v>0</v>
+      </c>
+      <c r="I686" t="s">
+        <v>57</v>
+      </c>
+      <c r="J686" t="s">
+        <v>86</v>
+      </c>
+      <c r="K686" t="s">
+        <v>39</v>
+      </c>
+      <c r="L686" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="687" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A687" t="s">
+        <v>1</v>
+      </c>
+      <c r="B687">
+        <v>2024</v>
+      </c>
+      <c r="C687" s="1">
+        <v>5</v>
+      </c>
+      <c r="D687" s="1">
+        <v>2</v>
+      </c>
+      <c r="E687">
+        <v>14471.975813620307</v>
+      </c>
+      <c r="F687">
+        <v>15769.519127953165</v>
+      </c>
+      <c r="G687">
+        <v>0</v>
+      </c>
+      <c r="H687">
+        <v>0</v>
+      </c>
+      <c r="I687" t="s">
+        <v>57</v>
+      </c>
+      <c r="J687" t="s">
+        <v>86</v>
+      </c>
+      <c r="K687" t="s">
+        <v>39</v>
+      </c>
+      <c r="L687" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="688" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A688" t="s">
+        <v>1</v>
+      </c>
+      <c r="B688">
+        <v>2024</v>
+      </c>
+      <c r="C688" s="1">
+        <v>5</v>
+      </c>
+      <c r="D688" s="1">
+        <v>3</v>
+      </c>
+      <c r="E688">
+        <v>1090.515511575815</v>
+      </c>
+      <c r="F688">
+        <v>3124.6854585110136</v>
+      </c>
+      <c r="G688">
+        <v>0</v>
+      </c>
+      <c r="H688">
+        <v>0</v>
+      </c>
+      <c r="I688" t="s">
+        <v>57</v>
+      </c>
+      <c r="J688" t="s">
+        <v>86</v>
+      </c>
+      <c r="K688" t="s">
+        <v>39</v>
+      </c>
+      <c r="L688" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="689" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A689" t="s">
+        <v>1</v>
+      </c>
+      <c r="B689">
+        <v>2024</v>
+      </c>
+      <c r="C689" s="1">
+        <v>6</v>
+      </c>
+      <c r="D689" s="1">
+        <v>3</v>
+      </c>
+      <c r="E689">
+        <v>400.29763393037445</v>
+      </c>
+      <c r="F689">
+        <v>55.316639130895297</v>
+      </c>
+      <c r="G689">
+        <v>0</v>
+      </c>
+      <c r="H689">
+        <v>0</v>
+      </c>
+      <c r="I689" t="s">
+        <v>57</v>
+      </c>
+      <c r="J689" t="s">
+        <v>86</v>
+      </c>
+      <c r="K689" t="s">
+        <v>39</v>
+      </c>
+      <c r="L689" t="s">
         <v>41</v>
       </c>
     </row>
@@ -25716,11 +26178,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A94BF84-AB01-45F2-8A1E-DD5B502642C6}">
-  <dimension ref="A1:T126"/>
+  <dimension ref="A1:T127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q92" sqref="Q92"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25795,6 +26257,9 @@
       <c r="A2">
         <v>1915</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2">
         <v>7400000</v>
       </c>
@@ -25803,6 +26268,9 @@
       <c r="A3">
         <v>1916</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
       <c r="E3">
         <v>4078000</v>
       </c>
@@ -25811,6 +26279,9 @@
       <c r="A4">
         <v>1917</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
       <c r="E4">
         <v>6995075</v>
       </c>
@@ -31132,6 +31603,65 @@
         <v>41</v>
       </c>
       <c r="T126" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>2024</v>
+      </c>
+      <c r="B127">
+        <v>3537</v>
+      </c>
+      <c r="C127">
+        <v>4769</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127" s="6">
+        <v>0</v>
+      </c>
+      <c r="F127" s="6">
+        <v>0</v>
+      </c>
+      <c r="G127" t="s">
+        <v>6</v>
+      </c>
+      <c r="H127">
+        <v>86</v>
+      </c>
+      <c r="I127">
+        <v>8.4276426679508784E-4</v>
+      </c>
+      <c r="J127">
+        <v>0.32915964363111005</v>
+      </c>
+      <c r="K127">
+        <v>0.53720202263424033</v>
+      </c>
+      <c r="L127">
+        <v>0</v>
+      </c>
+      <c r="M127">
+        <v>0</v>
+      </c>
+      <c r="N127">
+        <v>0.13279556946785456</v>
+      </c>
+      <c r="O127">
+        <v>0</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>44</v>
+      </c>
+      <c r="R127" t="s">
+        <v>86</v>
+      </c>
+      <c r="S127" t="s">
+        <v>41</v>
+      </c>
+      <c r="T127" t="s">
         <v>39</v>
       </c>
     </row>
@@ -40256,8 +40786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F161B800-98B7-4043-8D52-286424C777BB}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40931,7 +41461,7 @@
         <v>115</v>
       </c>
       <c r="D48">
-        <v>3004</v>
+        <v>3047</v>
       </c>
     </row>
   </sheetData>
@@ -40946,6 +41476,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000614419EC33FAD42A0282CFF32600A20" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8b94ec4c5b022f3c1dd5ef88a1c70be4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d4f3f700-51b4-43ff-b002-6ed848604d46" xmlns:ns3="01f01bef-47b7-4725-adaf-9b6a8bd74ef4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0d993d6f0fe140b5b27b8bdb1a11ff43" ns2:_="" ns3:_="">
     <xsd:import namespace="d4f3f700-51b4-43ff-b002-6ed848604d46"/>
@@ -41154,15 +41693,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22AD2C85-521D-4770-88CD-9DAE105CB1B6}">
   <ds:schemaRefs>
@@ -41173,6 +41703,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{729962EC-F35D-459B-8881-4F6AA84AC69F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83F8A5F1-9F5C-410C-A02F-9F6149407001}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41189,12 +41727,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{729962EC-F35D-459B-8881-4F6AA84AC69F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>